<commit_message>
Major Update Prior to Submission
Changes to multiple files to tidy up items prior to submission of the
project.
Major change to RLS program too. Note, still not working!
</commit_message>
<xml_diff>
--- a/docs/analysis/Step Test Continuity.xlsx
+++ b/docs/analysis/Step Test Continuity.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l1124010\Downloads\researchProject-master\researchProject-master\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\researchProject\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -156,7 +156,15 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>OP</c:v>
+            <c:strRef>
+              <c:f>'35-40'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -184,10 +192,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'35-40'!$A$4:$A$159</c:f>
+              <c:f>'35-40'!$A$4:$A$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="156"/>
+                <c:ptCount val="126"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -565,573 +573,393 @@
                 </c:pt>
                 <c:pt idx="125">
                   <c:v>1260</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>1270</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>1280</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>1290</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>1310</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>1320</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>1330</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>1340</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>1360</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>1370</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>1380</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>1390</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>1410</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>1420</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>1430</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>1440</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>1450</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>1460</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>1470</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>1480</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>1490</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>1510</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>1520</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>1530</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>1540</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>1550</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>1560</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'35-40'!$D$4:$D$159</c:f>
+              <c:f>'35-40'!$D$4:$D$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="156"/>
+                <c:ptCount val="126"/>
                 <c:pt idx="0">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>400</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1142,7 +970,15 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>03.11.15</c:v>
+            <c:strRef>
+              <c:f>'35-40'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PV 03/11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1170,10 +1006,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'35-40'!$A$4:$A$159</c:f>
+              <c:f>'35-40'!$A$4:$A$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="156"/>
+                <c:ptCount val="126"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1551,573 +1387,393 @@
                 </c:pt>
                 <c:pt idx="125">
                   <c:v>1260</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>1270</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>1280</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>1290</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>1310</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>1320</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>1330</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>1340</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>1360</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>1370</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>1380</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>1390</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>1410</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>1420</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>1430</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>1440</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>1450</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>1460</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>1470</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>1480</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>1490</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>1510</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>1520</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>1530</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>1540</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>1550</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>1560</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'35-40'!$B$4:$B$159</c:f>
+              <c:f>'35-40'!$B$4:$B$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="156"/>
+                <c:ptCount val="126"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>93</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>87</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>94</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>91</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>97</c:v>
+                  <c:v>9.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104</c:v>
+                  <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>109</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>115</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>123</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>126</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>134</c:v>
+                  <c:v>13.4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>131</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>146</c:v>
+                  <c:v>14.6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>149</c:v>
+                  <c:v>14.9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>154</c:v>
+                  <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>163</c:v>
+                  <c:v>16.3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>170</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>178</c:v>
+                  <c:v>17.8</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>180</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>180</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>193</c:v>
+                  <c:v>19.3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>194</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>203</c:v>
+                  <c:v>20.3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>209</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>212</c:v>
+                  <c:v>21.2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>210</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>218</c:v>
+                  <c:v>21.8</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>230</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>239</c:v>
+                  <c:v>23.9</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>240</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>241</c:v>
+                  <c:v>24.1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>245</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>247</c:v>
+                  <c:v>24.7</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>251</c:v>
+                  <c:v>25.1</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>263</c:v>
+                  <c:v>26.3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>259</c:v>
+                  <c:v>25.9</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>271</c:v>
+                  <c:v>27.1</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>273</c:v>
+                  <c:v>27.3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>274</c:v>
+                  <c:v>27.4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>278</c:v>
+                  <c:v>27.8</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>284</c:v>
+                  <c:v>28.4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>281</c:v>
+                  <c:v>28.1</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>294</c:v>
+                  <c:v>29.4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>298</c:v>
+                  <c:v>29.8</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>302</c:v>
+                  <c:v>30.2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>303</c:v>
+                  <c:v>30.3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>305</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>308</c:v>
+                  <c:v>30.8</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>309</c:v>
+                  <c:v>30.9</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>320</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>321</c:v>
+                  <c:v>32.1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>322</c:v>
+                  <c:v>32.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>326</c:v>
+                  <c:v>32.6</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>327</c:v>
+                  <c:v>32.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>333</c:v>
+                  <c:v>33.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>336</c:v>
+                  <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>337</c:v>
+                  <c:v>33.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>343</c:v>
+                  <c:v>34.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>350</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>352</c:v>
+                  <c:v>35.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>353</c:v>
+                  <c:v>35.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>358</c:v>
+                  <c:v>35.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>358</c:v>
+                  <c:v>35.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>363</c:v>
+                  <c:v>36.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>366</c:v>
+                  <c:v>36.6</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>365</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>367</c:v>
+                  <c:v>36.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>367</c:v>
+                  <c:v>36.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>372</c:v>
+                  <c:v>37.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>376</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>374</c:v>
+                  <c:v>37.4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>382</c:v>
+                  <c:v>38.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>378</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>387</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>388</c:v>
+                  <c:v>38.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>389</c:v>
+                  <c:v>38.9</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>392</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>394</c:v>
+                  <c:v>39.4</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>397</c:v>
+                  <c:v>39.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>399</c:v>
+                  <c:v>39.9</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>402</c:v>
+                  <c:v>40.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>396</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>402</c:v>
+                  <c:v>40.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>401</c:v>
+                  <c:v>40.1</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>403</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>407</c:v>
+                  <c:v>40.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>410</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>415</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>421</c:v>
+                  <c:v>42.1</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>423</c:v>
+                  <c:v>42.3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>418</c:v>
+                  <c:v>41.8</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>418</c:v>
+                  <c:v>41.8</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>427</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>427</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>427</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>426</c:v>
+                  <c:v>42.6</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>426</c:v>
+                  <c:v>42.6</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>429</c:v>
+                  <c:v>42.9</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>429</c:v>
+                  <c:v>42.9</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>432</c:v>
+                  <c:v>43.2</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>427</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>429</c:v>
+                  <c:v>42.9</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>429</c:v>
+                  <c:v>42.9</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>430</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>432</c:v>
+                  <c:v>43.2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>434</c:v>
+                  <c:v>43.4</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>434</c:v>
+                  <c:v>43.4</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>433</c:v>
+                  <c:v>43.3</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>436</c:v>
+                  <c:v>43.6</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>437</c:v>
+                  <c:v>43.7</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>447</c:v>
+                  <c:v>44.7</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>448</c:v>
+                  <c:v>44.8</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>436</c:v>
+                  <c:v>43.6</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>442</c:v>
+                  <c:v>44.2</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>454</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>446</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>445</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>452</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>447</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>456</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>454</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>456</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>457</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>458</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>457</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>463</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>463</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>466</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>465</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>458</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>467</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>463</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>464</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>464</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>471</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>466</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>469</c:v>
+                  <c:v>45.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2128,7 +1784,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>04.11.15</c:v>
+            <c:strRef>
+              <c:f>'35-40'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PV 04/11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
@@ -2524,382 +2188,382 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="126"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>96</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97</c:v>
+                  <c:v>9.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>94</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>88</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>85</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>87</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>93</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104</c:v>
+                  <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>110</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>114</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>122</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>130</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>130</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>138</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>144</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>151</c:v>
+                  <c:v>15.1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>155</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>165</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>173</c:v>
+                  <c:v>17.3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>177</c:v>
+                  <c:v>17.7</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>179</c:v>
+                  <c:v>17.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>183</c:v>
+                  <c:v>18.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>192</c:v>
+                  <c:v>19.2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>200</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>208</c:v>
+                  <c:v>20.8</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>207</c:v>
+                  <c:v>20.7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>211</c:v>
+                  <c:v>21.1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>223</c:v>
+                  <c:v>22.3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>225</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>230</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>237</c:v>
+                  <c:v>23.7</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>238</c:v>
+                  <c:v>23.8</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>249</c:v>
+                  <c:v>24.9</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>252</c:v>
+                  <c:v>25.2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>261</c:v>
+                  <c:v>26.1</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>266</c:v>
+                  <c:v>26.6</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>263</c:v>
+                  <c:v>26.3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>268</c:v>
+                  <c:v>26.8</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>270</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>274</c:v>
+                  <c:v>27.4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>284</c:v>
+                  <c:v>28.4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>292</c:v>
+                  <c:v>29.2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>298</c:v>
+                  <c:v>29.8</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>300</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>305</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>301</c:v>
+                  <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>307</c:v>
+                  <c:v>30.7</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>303</c:v>
+                  <c:v>30.3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>314</c:v>
+                  <c:v>31.4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>317</c:v>
+                  <c:v>31.7</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>326</c:v>
+                  <c:v>32.6</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>328</c:v>
+                  <c:v>32.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>328</c:v>
+                  <c:v>32.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>331</c:v>
+                  <c:v>33.1</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>330</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>332</c:v>
+                  <c:v>33.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>338</c:v>
+                  <c:v>33.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>342</c:v>
+                  <c:v>34.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>343</c:v>
+                  <c:v>34.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>351</c:v>
+                  <c:v>35.1</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>355</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>357</c:v>
+                  <c:v>35.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>354</c:v>
+                  <c:v>35.4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>360</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>360</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>366</c:v>
+                  <c:v>36.6</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>366</c:v>
+                  <c:v>36.6</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>371</c:v>
+                  <c:v>37.1</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>368</c:v>
+                  <c:v>36.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>371</c:v>
+                  <c:v>37.1</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>371</c:v>
+                  <c:v>37.1</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>380</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>381</c:v>
+                  <c:v>38.1</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>389</c:v>
+                  <c:v>38.9</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>389</c:v>
+                  <c:v>38.9</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>392</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>388</c:v>
+                  <c:v>38.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>393</c:v>
+                  <c:v>39.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>397</c:v>
+                  <c:v>39.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>398</c:v>
+                  <c:v>39.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>398</c:v>
+                  <c:v>39.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>402</c:v>
+                  <c:v>40.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>399</c:v>
+                  <c:v>39.9</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>406</c:v>
+                  <c:v>40.6</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>411</c:v>
+                  <c:v>41.1</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>411</c:v>
+                  <c:v>41.1</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>417</c:v>
+                  <c:v>41.7</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>416</c:v>
+                  <c:v>41.6</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>416</c:v>
+                  <c:v>41.6</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>420</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>422</c:v>
+                  <c:v>42.2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>422</c:v>
+                  <c:v>42.2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>424</c:v>
+                  <c:v>42.4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>423</c:v>
+                  <c:v>42.3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>424</c:v>
+                  <c:v>42.4</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>426</c:v>
+                  <c:v>42.6</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>428</c:v>
+                  <c:v>42.8</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>428</c:v>
+                  <c:v>42.8</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>428</c:v>
+                  <c:v>42.8</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>428</c:v>
+                  <c:v>42.8</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>430</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>433</c:v>
+                  <c:v>43.3</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>436</c:v>
+                  <c:v>43.6</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>428</c:v>
+                  <c:v>42.8</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>430</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>438</c:v>
+                  <c:v>43.8</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>441</c:v>
+                  <c:v>44.1</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>447</c:v>
+                  <c:v>44.7</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>447</c:v>
+                  <c:v>44.7</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>444</c:v>
+                  <c:v>44.4</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>449</c:v>
+                  <c:v>44.9</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>451</c:v>
+                  <c:v>45.1</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>452</c:v>
+                  <c:v>45.2</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>448</c:v>
+                  <c:v>44.8</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>453</c:v>
+                  <c:v>45.3</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>455</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>454</c:v>
+                  <c:v>45.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2914,14 +2578,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="570348816"/>
-        <c:axId val="570553800"/>
+        <c:axId val="430725232"/>
+        <c:axId val="430722992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570348816"/>
+        <c:axId val="430725232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1600"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2939,6 +2602,25 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2976,12 +2658,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570553800"/>
+        <c:crossAx val="430722992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570553800"/>
+        <c:axId val="430722992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3001,6 +2683,30 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>PV</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>, OP (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3038,7 +2744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570348816"/>
+        <c:crossAx val="430725232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3096,16 +2802,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>609597</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114297</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>611604</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>116304</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>5013</xdr:rowOff>
+      <xdr:rowOff>119313</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3414,10 +3120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3449,13 +3155,13 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>104</v>
+        <v>10.4</v>
       </c>
       <c r="D4">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3464,13 +3170,13 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>89</v>
+        <v>8.9</v>
       </c>
       <c r="D5">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3479,13 +3185,13 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>91</v>
+        <v>9.1</v>
       </c>
       <c r="C6">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3494,13 +3200,13 @@
         <v>40</v>
       </c>
       <c r="B7">
-        <v>87</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C7">
-        <v>92</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D7">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3509,13 +3215,13 @@
         <v>50</v>
       </c>
       <c r="B8">
-        <v>95</v>
+        <v>9.5</v>
       </c>
       <c r="C8">
-        <v>89</v>
+        <v>8.9</v>
       </c>
       <c r="D8">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3524,13 +3230,13 @@
         <v>60</v>
       </c>
       <c r="B9">
-        <v>93</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C9">
-        <v>86</v>
+        <v>8.6</v>
       </c>
       <c r="D9">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3539,13 +3245,13 @@
         <v>70</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>92</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D10">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,13 +3260,13 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <v>87</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C11">
-        <v>96</v>
+        <v>9.6</v>
       </c>
       <c r="D11">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3569,13 +3275,13 @@
         <v>90</v>
       </c>
       <c r="B12">
-        <v>93</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C12">
-        <v>97</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D12">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,13 +3290,13 @@
         <v>100</v>
       </c>
       <c r="B13">
-        <v>86</v>
+        <v>8.6</v>
       </c>
       <c r="C13">
-        <v>94</v>
+        <v>9.4</v>
       </c>
       <c r="D13">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3599,13 +3305,13 @@
         <v>110</v>
       </c>
       <c r="B14">
-        <v>87</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C14">
-        <v>96</v>
+        <v>9.6</v>
       </c>
       <c r="D14">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3614,13 +3320,13 @@
         <v>120</v>
       </c>
       <c r="B15">
-        <v>94</v>
+        <v>9.4</v>
       </c>
       <c r="C15">
-        <v>92</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D15">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3629,13 +3335,13 @@
         <v>130</v>
       </c>
       <c r="B16">
-        <v>91</v>
+        <v>9.1</v>
       </c>
       <c r="C16">
-        <v>88</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D16">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3644,13 +3350,13 @@
         <v>140</v>
       </c>
       <c r="B17">
-        <v>91</v>
+        <v>9.1</v>
       </c>
       <c r="C17">
-        <v>85</v>
+        <v>8.5</v>
       </c>
       <c r="D17">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3659,13 +3365,13 @@
         <v>150</v>
       </c>
       <c r="B18">
-        <v>97</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C18">
-        <v>87</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D18">
-        <v>350</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3674,13 +3380,13 @@
         <v>160</v>
       </c>
       <c r="B19">
-        <v>92</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C19">
-        <v>93</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D19">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3689,13 +3395,13 @@
         <v>170</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>10.4</v>
       </c>
       <c r="C20">
-        <v>104</v>
+        <v>10.4</v>
       </c>
       <c r="D20">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3704,13 +3410,13 @@
         <v>180</v>
       </c>
       <c r="B21">
-        <v>109</v>
+        <v>10.9</v>
       </c>
       <c r="C21">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3719,13 +3425,13 @@
         <v>190</v>
       </c>
       <c r="B22">
-        <v>115</v>
+        <v>11.5</v>
       </c>
       <c r="C22">
-        <v>114</v>
+        <v>11.4</v>
       </c>
       <c r="D22">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3734,13 +3440,13 @@
         <v>200</v>
       </c>
       <c r="B23">
-        <v>123</v>
+        <v>12.3</v>
       </c>
       <c r="C23">
-        <v>122</v>
+        <v>12.2</v>
       </c>
       <c r="D23">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,13 +3455,13 @@
         <v>210</v>
       </c>
       <c r="B24">
-        <v>126</v>
+        <v>12.6</v>
       </c>
       <c r="C24">
-        <v>130</v>
+        <v>13</v>
       </c>
       <c r="D24">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3764,13 +3470,13 @@
         <v>220</v>
       </c>
       <c r="B25">
-        <v>134</v>
+        <v>13.4</v>
       </c>
       <c r="C25">
-        <v>130</v>
+        <v>13</v>
       </c>
       <c r="D25">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3779,13 +3485,13 @@
         <v>230</v>
       </c>
       <c r="B26">
-        <v>131</v>
+        <v>13.1</v>
       </c>
       <c r="C26">
-        <v>138</v>
+        <v>13.8</v>
       </c>
       <c r="D26">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3794,13 +3500,13 @@
         <v>240</v>
       </c>
       <c r="B27">
-        <v>146</v>
+        <v>14.6</v>
       </c>
       <c r="C27">
-        <v>144</v>
+        <v>14.4</v>
       </c>
       <c r="D27">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3809,13 +3515,13 @@
         <v>250</v>
       </c>
       <c r="B28">
-        <v>149</v>
+        <v>14.9</v>
       </c>
       <c r="C28">
-        <v>151</v>
+        <v>15.1</v>
       </c>
       <c r="D28">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3824,13 +3530,13 @@
         <v>260</v>
       </c>
       <c r="B29">
-        <v>154</v>
+        <v>15.4</v>
       </c>
       <c r="C29">
-        <v>155</v>
+        <v>15.5</v>
       </c>
       <c r="D29">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3839,13 +3545,13 @@
         <v>270</v>
       </c>
       <c r="B30">
-        <v>163</v>
+        <v>16.3</v>
       </c>
       <c r="C30">
-        <v>165</v>
+        <v>16.5</v>
       </c>
       <c r="D30">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3854,13 +3560,13 @@
         <v>280</v>
       </c>
       <c r="B31">
-        <v>170</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>173</v>
+        <v>17.3</v>
       </c>
       <c r="D31">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3869,13 +3575,13 @@
         <v>290</v>
       </c>
       <c r="B32">
-        <v>178</v>
+        <v>17.8</v>
       </c>
       <c r="C32">
-        <v>177</v>
+        <v>17.7</v>
       </c>
       <c r="D32">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3884,13 +3590,13 @@
         <v>300</v>
       </c>
       <c r="B33">
-        <v>180</v>
+        <v>18</v>
       </c>
       <c r="C33">
-        <v>179</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="D33">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3899,13 +3605,13 @@
         <v>310</v>
       </c>
       <c r="B34">
-        <v>180</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>183</v>
+        <v>18.3</v>
       </c>
       <c r="D34">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3914,13 +3620,13 @@
         <v>320</v>
       </c>
       <c r="B35">
-        <v>193</v>
+        <v>19.3</v>
       </c>
       <c r="C35">
-        <v>192</v>
+        <v>19.2</v>
       </c>
       <c r="D35">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,13 +3635,13 @@
         <v>330</v>
       </c>
       <c r="B36">
-        <v>194</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="C36">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D36">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3944,13 +3650,13 @@
         <v>340</v>
       </c>
       <c r="B37">
-        <v>203</v>
+        <v>20.3</v>
       </c>
       <c r="C37">
-        <v>208</v>
+        <v>20.8</v>
       </c>
       <c r="D37">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3959,13 +3665,13 @@
         <v>350</v>
       </c>
       <c r="B38">
-        <v>209</v>
+        <v>20.9</v>
       </c>
       <c r="C38">
-        <v>207</v>
+        <v>20.7</v>
       </c>
       <c r="D38">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3974,13 +3680,13 @@
         <v>360</v>
       </c>
       <c r="B39">
-        <v>212</v>
+        <v>21.2</v>
       </c>
       <c r="C39">
-        <v>211</v>
+        <v>21.1</v>
       </c>
       <c r="D39">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3989,13 +3695,13 @@
         <v>370</v>
       </c>
       <c r="B40">
-        <v>210</v>
+        <v>21</v>
       </c>
       <c r="C40">
-        <v>223</v>
+        <v>22.3</v>
       </c>
       <c r="D40">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4004,13 +3710,13 @@
         <v>380</v>
       </c>
       <c r="B41">
-        <v>218</v>
+        <v>21.8</v>
       </c>
       <c r="C41">
-        <v>225</v>
+        <v>22.5</v>
       </c>
       <c r="D41">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4019,13 +3725,13 @@
         <v>390</v>
       </c>
       <c r="B42">
-        <v>230</v>
+        <v>23</v>
       </c>
       <c r="C42">
-        <v>230</v>
+        <v>23</v>
       </c>
       <c r="D42">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4034,13 +3740,13 @@
         <v>400</v>
       </c>
       <c r="B43">
-        <v>239</v>
+        <v>23.9</v>
       </c>
       <c r="C43">
-        <v>237</v>
+        <v>23.7</v>
       </c>
       <c r="D43">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4049,13 +3755,13 @@
         <v>410</v>
       </c>
       <c r="B44">
-        <v>240</v>
+        <v>24</v>
       </c>
       <c r="C44">
-        <v>238</v>
+        <v>23.8</v>
       </c>
       <c r="D44">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4064,13 +3770,13 @@
         <v>420</v>
       </c>
       <c r="B45">
-        <v>241</v>
+        <v>24.1</v>
       </c>
       <c r="C45">
-        <v>249</v>
+        <v>24.9</v>
       </c>
       <c r="D45">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4079,13 +3785,13 @@
         <v>430</v>
       </c>
       <c r="B46">
-        <v>245</v>
+        <v>24.5</v>
       </c>
       <c r="C46">
-        <v>252</v>
+        <v>25.2</v>
       </c>
       <c r="D46">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4094,13 +3800,13 @@
         <v>440</v>
       </c>
       <c r="B47">
-        <v>247</v>
+        <v>24.7</v>
       </c>
       <c r="C47">
-        <v>261</v>
+        <v>26.1</v>
       </c>
       <c r="D47">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4109,13 +3815,13 @@
         <v>450</v>
       </c>
       <c r="B48">
-        <v>251</v>
+        <v>25.1</v>
       </c>
       <c r="C48">
-        <v>266</v>
+        <v>26.6</v>
       </c>
       <c r="D48">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4124,13 +3830,13 @@
         <v>460</v>
       </c>
       <c r="B49">
-        <v>263</v>
+        <v>26.3</v>
       </c>
       <c r="C49">
-        <v>263</v>
+        <v>26.3</v>
       </c>
       <c r="D49">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4139,13 +3845,13 @@
         <v>470</v>
       </c>
       <c r="B50">
-        <v>259</v>
+        <v>25.9</v>
       </c>
       <c r="C50">
-        <v>268</v>
+        <v>26.8</v>
       </c>
       <c r="D50">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4154,13 +3860,13 @@
         <v>480</v>
       </c>
       <c r="B51">
-        <v>271</v>
+        <v>27.1</v>
       </c>
       <c r="C51">
-        <v>270</v>
+        <v>27</v>
       </c>
       <c r="D51">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4169,13 +3875,13 @@
         <v>490</v>
       </c>
       <c r="B52">
-        <v>273</v>
+        <v>27.3</v>
       </c>
       <c r="C52">
-        <v>274</v>
+        <v>27.4</v>
       </c>
       <c r="D52">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4184,13 +3890,13 @@
         <v>500</v>
       </c>
       <c r="B53">
-        <v>274</v>
+        <v>27.4</v>
       </c>
       <c r="C53">
-        <v>284</v>
+        <v>28.4</v>
       </c>
       <c r="D53">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4199,13 +3905,13 @@
         <v>510</v>
       </c>
       <c r="B54">
-        <v>278</v>
+        <v>27.8</v>
       </c>
       <c r="C54">
-        <v>292</v>
+        <v>29.2</v>
       </c>
       <c r="D54">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4214,13 +3920,13 @@
         <v>520</v>
       </c>
       <c r="B55">
-        <v>284</v>
+        <v>28.4</v>
       </c>
       <c r="C55">
-        <v>298</v>
+        <v>29.8</v>
       </c>
       <c r="D55">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4229,13 +3935,13 @@
         <v>530</v>
       </c>
       <c r="B56">
-        <v>281</v>
+        <v>28.1</v>
       </c>
       <c r="C56">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="D56">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4244,13 +3950,13 @@
         <v>540</v>
       </c>
       <c r="B57">
-        <v>294</v>
+        <v>29.4</v>
       </c>
       <c r="C57">
-        <v>305</v>
+        <v>30.5</v>
       </c>
       <c r="D57">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4259,13 +3965,13 @@
         <v>550</v>
       </c>
       <c r="B58">
-        <v>298</v>
+        <v>29.8</v>
       </c>
       <c r="C58">
-        <v>301</v>
+        <v>30.1</v>
       </c>
       <c r="D58">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4274,13 +3980,13 @@
         <v>560</v>
       </c>
       <c r="B59">
-        <v>302</v>
+        <v>30.2</v>
       </c>
       <c r="C59">
-        <v>307</v>
+        <v>30.7</v>
       </c>
       <c r="D59">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4289,13 +3995,13 @@
         <v>570</v>
       </c>
       <c r="B60">
-        <v>303</v>
+        <v>30.3</v>
       </c>
       <c r="C60">
-        <v>303</v>
+        <v>30.3</v>
       </c>
       <c r="D60">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4304,13 +4010,13 @@
         <v>580</v>
       </c>
       <c r="B61">
-        <v>305</v>
+        <v>30.5</v>
       </c>
       <c r="C61">
-        <v>314</v>
+        <v>31.4</v>
       </c>
       <c r="D61">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4319,13 +4025,13 @@
         <v>590</v>
       </c>
       <c r="B62">
-        <v>308</v>
+        <v>30.8</v>
       </c>
       <c r="C62">
-        <v>317</v>
+        <v>31.7</v>
       </c>
       <c r="D62">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4334,13 +4040,13 @@
         <v>600</v>
       </c>
       <c r="B63">
-        <v>309</v>
+        <v>30.9</v>
       </c>
       <c r="C63">
-        <v>326</v>
+        <v>32.6</v>
       </c>
       <c r="D63">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4349,13 +4055,13 @@
         <v>610</v>
       </c>
       <c r="B64">
-        <v>320</v>
+        <v>32</v>
       </c>
       <c r="C64">
-        <v>328</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="D64">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4364,13 +4070,13 @@
         <v>620</v>
       </c>
       <c r="B65">
-        <v>321</v>
+        <v>32.1</v>
       </c>
       <c r="C65">
-        <v>328</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="D65">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4379,13 +4085,13 @@
         <v>630</v>
       </c>
       <c r="B66">
-        <v>322</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="C66">
-        <v>331</v>
+        <v>33.1</v>
       </c>
       <c r="D66">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4394,13 +4100,13 @@
         <v>640</v>
       </c>
       <c r="B67">
-        <v>326</v>
+        <v>32.6</v>
       </c>
       <c r="C67">
-        <v>330</v>
+        <v>33</v>
       </c>
       <c r="D67">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4409,13 +4115,13 @@
         <v>650</v>
       </c>
       <c r="B68">
-        <v>327</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="C68">
-        <v>332</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="D68">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4424,28 +4130,28 @@
         <v>660</v>
       </c>
       <c r="B69">
-        <v>333</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="C69">
-        <v>338</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="D69">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" ref="A70:A133" si="1">A69+10</f>
+        <f t="shared" ref="A70:A129" si="1">A69+10</f>
         <v>670</v>
       </c>
       <c r="B70">
-        <v>336</v>
+        <v>33.6</v>
       </c>
       <c r="C70">
-        <v>342</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="D70">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4454,13 +4160,13 @@
         <v>680</v>
       </c>
       <c r="B71">
-        <v>337</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="C71">
-        <v>343</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D71">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4469,13 +4175,13 @@
         <v>690</v>
       </c>
       <c r="B72">
-        <v>343</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="C72">
-        <v>351</v>
+        <v>35.1</v>
       </c>
       <c r="D72">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4484,13 +4190,13 @@
         <v>700</v>
       </c>
       <c r="B73">
-        <v>350</v>
+        <v>35</v>
       </c>
       <c r="C73">
-        <v>355</v>
+        <v>35.5</v>
       </c>
       <c r="D73">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4499,13 +4205,13 @@
         <v>710</v>
       </c>
       <c r="B74">
-        <v>352</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="C74">
-        <v>357</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="D74">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4514,13 +4220,13 @@
         <v>720</v>
       </c>
       <c r="B75">
-        <v>353</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="C75">
-        <v>354</v>
+        <v>35.4</v>
       </c>
       <c r="D75">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4529,13 +4235,13 @@
         <v>730</v>
       </c>
       <c r="B76">
-        <v>358</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="C76">
-        <v>360</v>
+        <v>36</v>
       </c>
       <c r="D76">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4544,13 +4250,13 @@
         <v>740</v>
       </c>
       <c r="B77">
-        <v>358</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="C77">
-        <v>360</v>
+        <v>36</v>
       </c>
       <c r="D77">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4559,13 +4265,13 @@
         <v>750</v>
       </c>
       <c r="B78">
-        <v>363</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="C78">
-        <v>366</v>
+        <v>36.6</v>
       </c>
       <c r="D78">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4574,13 +4280,13 @@
         <v>760</v>
       </c>
       <c r="B79">
-        <v>366</v>
+        <v>36.6</v>
       </c>
       <c r="C79">
-        <v>366</v>
+        <v>36.6</v>
       </c>
       <c r="D79">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4589,13 +4295,13 @@
         <v>770</v>
       </c>
       <c r="B80">
-        <v>365</v>
+        <v>36.5</v>
       </c>
       <c r="C80">
-        <v>371</v>
+        <v>37.1</v>
       </c>
       <c r="D80">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4604,13 +4310,13 @@
         <v>780</v>
       </c>
       <c r="B81">
-        <v>367</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="C81">
-        <v>368</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="D81">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4619,13 +4325,13 @@
         <v>790</v>
       </c>
       <c r="B82">
-        <v>367</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="C82">
-        <v>371</v>
+        <v>37.1</v>
       </c>
       <c r="D82">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4634,13 +4340,13 @@
         <v>800</v>
       </c>
       <c r="B83">
-        <v>372</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="C83">
-        <v>371</v>
+        <v>37.1</v>
       </c>
       <c r="D83">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4649,13 +4355,13 @@
         <v>810</v>
       </c>
       <c r="B84">
-        <v>376</v>
+        <v>37.6</v>
       </c>
       <c r="C84">
-        <v>380</v>
+        <v>38</v>
       </c>
       <c r="D84">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4664,13 +4370,13 @@
         <v>820</v>
       </c>
       <c r="B85">
-        <v>374</v>
+        <v>37.4</v>
       </c>
       <c r="C85">
-        <v>381</v>
+        <v>38.1</v>
       </c>
       <c r="D85">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4679,13 +4385,13 @@
         <v>830</v>
       </c>
       <c r="B86">
-        <v>382</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="C86">
-        <v>389</v>
+        <v>38.9</v>
       </c>
       <c r="D86">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4694,13 +4400,13 @@
         <v>840</v>
       </c>
       <c r="B87">
-        <v>378</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="C87">
-        <v>389</v>
+        <v>38.9</v>
       </c>
       <c r="D87">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4709,13 +4415,13 @@
         <v>850</v>
       </c>
       <c r="B88">
-        <v>387</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="C88">
-        <v>392</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="D88">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4724,13 +4430,13 @@
         <v>860</v>
       </c>
       <c r="B89">
-        <v>388</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="C89">
-        <v>388</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="D89">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4739,13 +4445,13 @@
         <v>870</v>
       </c>
       <c r="B90">
-        <v>389</v>
+        <v>38.9</v>
       </c>
       <c r="C90">
-        <v>393</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="D90">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4754,13 +4460,13 @@
         <v>880</v>
       </c>
       <c r="B91">
-        <v>392</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="C91">
-        <v>397</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="D91">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4769,13 +4475,13 @@
         <v>890</v>
       </c>
       <c r="B92">
-        <v>394</v>
+        <v>39.4</v>
       </c>
       <c r="C92">
-        <v>398</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="D92">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4784,13 +4490,13 @@
         <v>900</v>
       </c>
       <c r="B93">
-        <v>397</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="C93">
-        <v>398</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="D93">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4799,13 +4505,13 @@
         <v>910</v>
       </c>
       <c r="B94">
-        <v>399</v>
+        <v>39.9</v>
       </c>
       <c r="C94">
-        <v>402</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="D94">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4814,13 +4520,13 @@
         <v>920</v>
       </c>
       <c r="B95">
-        <v>402</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="C95">
-        <v>399</v>
+        <v>39.9</v>
       </c>
       <c r="D95">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4829,13 +4535,13 @@
         <v>930</v>
       </c>
       <c r="B96">
-        <v>396</v>
+        <v>39.6</v>
       </c>
       <c r="C96">
-        <v>406</v>
+        <v>40.6</v>
       </c>
       <c r="D96">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4844,13 +4550,13 @@
         <v>940</v>
       </c>
       <c r="B97">
-        <v>402</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="C97">
-        <v>411</v>
+        <v>41.1</v>
       </c>
       <c r="D97">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4859,13 +4565,13 @@
         <v>950</v>
       </c>
       <c r="B98">
-        <v>401</v>
+        <v>40.1</v>
       </c>
       <c r="C98">
-        <v>411</v>
+        <v>41.1</v>
       </c>
       <c r="D98">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4874,13 +4580,13 @@
         <v>960</v>
       </c>
       <c r="B99">
-        <v>403</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="C99">
-        <v>417</v>
+        <v>41.7</v>
       </c>
       <c r="D99">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4889,13 +4595,13 @@
         <v>970</v>
       </c>
       <c r="B100">
-        <v>407</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="C100">
-        <v>416</v>
+        <v>41.6</v>
       </c>
       <c r="D100">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4904,13 +4610,13 @@
         <v>980</v>
       </c>
       <c r="B101">
-        <v>410</v>
+        <v>41</v>
       </c>
       <c r="C101">
-        <v>416</v>
+        <v>41.6</v>
       </c>
       <c r="D101">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4919,13 +4625,13 @@
         <v>990</v>
       </c>
       <c r="B102">
-        <v>415</v>
+        <v>41.5</v>
       </c>
       <c r="C102">
-        <v>420</v>
+        <v>42</v>
       </c>
       <c r="D102">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4934,13 +4640,13 @@
         <v>1000</v>
       </c>
       <c r="B103">
-        <v>421</v>
+        <v>42.1</v>
       </c>
       <c r="C103">
-        <v>422</v>
+        <v>42.2</v>
       </c>
       <c r="D103">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4949,13 +4655,13 @@
         <v>1010</v>
       </c>
       <c r="B104">
-        <v>423</v>
+        <v>42.3</v>
       </c>
       <c r="C104">
-        <v>422</v>
+        <v>42.2</v>
       </c>
       <c r="D104">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4964,13 +4670,13 @@
         <v>1020</v>
       </c>
       <c r="B105">
-        <v>418</v>
+        <v>41.8</v>
       </c>
       <c r="C105">
-        <v>424</v>
+        <v>42.4</v>
       </c>
       <c r="D105">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,13 +4685,13 @@
         <v>1030</v>
       </c>
       <c r="B106">
-        <v>418</v>
+        <v>41.8</v>
       </c>
       <c r="C106">
-        <v>423</v>
+        <v>42.3</v>
       </c>
       <c r="D106">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4994,13 +4700,13 @@
         <v>1040</v>
       </c>
       <c r="B107">
-        <v>427</v>
+        <v>42.7</v>
       </c>
       <c r="C107">
-        <v>424</v>
+        <v>42.4</v>
       </c>
       <c r="D107">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -5009,13 +4715,13 @@
         <v>1050</v>
       </c>
       <c r="B108">
-        <v>427</v>
+        <v>42.7</v>
       </c>
       <c r="C108">
-        <v>426</v>
+        <v>42.6</v>
       </c>
       <c r="D108">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5024,13 +4730,13 @@
         <v>1060</v>
       </c>
       <c r="B109">
-        <v>427</v>
+        <v>42.7</v>
       </c>
       <c r="C109">
-        <v>428</v>
+        <v>42.8</v>
       </c>
       <c r="D109">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -5039,13 +4745,13 @@
         <v>1070</v>
       </c>
       <c r="B110">
-        <v>426</v>
+        <v>42.6</v>
       </c>
       <c r="C110">
-        <v>428</v>
+        <v>42.8</v>
       </c>
       <c r="D110">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -5054,13 +4760,13 @@
         <v>1080</v>
       </c>
       <c r="B111">
-        <v>426</v>
+        <v>42.6</v>
       </c>
       <c r="C111">
-        <v>428</v>
+        <v>42.8</v>
       </c>
       <c r="D111">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -5069,13 +4775,13 @@
         <v>1090</v>
       </c>
       <c r="B112">
-        <v>429</v>
+        <v>42.9</v>
       </c>
       <c r="C112">
-        <v>428</v>
+        <v>42.8</v>
       </c>
       <c r="D112">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -5084,13 +4790,13 @@
         <v>1100</v>
       </c>
       <c r="B113">
-        <v>429</v>
+        <v>42.9</v>
       </c>
       <c r="C113">
-        <v>430</v>
+        <v>43</v>
       </c>
       <c r="D113">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -5099,13 +4805,13 @@
         <v>1110</v>
       </c>
       <c r="B114">
-        <v>432</v>
+        <v>43.2</v>
       </c>
       <c r="C114">
-        <v>433</v>
+        <v>43.3</v>
       </c>
       <c r="D114">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -5114,13 +4820,13 @@
         <v>1120</v>
       </c>
       <c r="B115">
-        <v>427</v>
+        <v>42.7</v>
       </c>
       <c r="C115">
-        <v>436</v>
+        <v>43.6</v>
       </c>
       <c r="D115">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -5129,13 +4835,13 @@
         <v>1130</v>
       </c>
       <c r="B116">
-        <v>429</v>
+        <v>42.9</v>
       </c>
       <c r="C116">
-        <v>428</v>
+        <v>42.8</v>
       </c>
       <c r="D116">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -5144,13 +4850,13 @@
         <v>1140</v>
       </c>
       <c r="B117">
-        <v>429</v>
+        <v>42.9</v>
       </c>
       <c r="C117">
-        <v>430</v>
+        <v>43</v>
       </c>
       <c r="D117">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5159,13 +4865,13 @@
         <v>1150</v>
       </c>
       <c r="B118">
-        <v>430</v>
+        <v>43</v>
       </c>
       <c r="C118">
-        <v>438</v>
+        <v>43.8</v>
       </c>
       <c r="D118">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5174,13 +4880,13 @@
         <v>1160</v>
       </c>
       <c r="B119">
-        <v>432</v>
+        <v>43.2</v>
       </c>
       <c r="C119">
-        <v>441</v>
+        <v>44.1</v>
       </c>
       <c r="D119">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5189,13 +4895,13 @@
         <v>1170</v>
       </c>
       <c r="B120">
-        <v>434</v>
+        <v>43.4</v>
       </c>
       <c r="C120">
-        <v>447</v>
+        <v>44.7</v>
       </c>
       <c r="D120">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5204,13 +4910,13 @@
         <v>1180</v>
       </c>
       <c r="B121">
-        <v>434</v>
+        <v>43.4</v>
       </c>
       <c r="C121">
-        <v>447</v>
+        <v>44.7</v>
       </c>
       <c r="D121">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -5219,13 +4925,13 @@
         <v>1190</v>
       </c>
       <c r="B122">
-        <v>433</v>
+        <v>43.3</v>
       </c>
       <c r="C122">
-        <v>444</v>
+        <v>44.4</v>
       </c>
       <c r="D122">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -5234,13 +4940,13 @@
         <v>1200</v>
       </c>
       <c r="B123">
-        <v>436</v>
+        <v>43.6</v>
       </c>
       <c r="C123">
-        <v>449</v>
+        <v>44.9</v>
       </c>
       <c r="D123">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5249,13 +4955,13 @@
         <v>1210</v>
       </c>
       <c r="B124">
-        <v>437</v>
+        <v>43.7</v>
       </c>
       <c r="C124">
-        <v>451</v>
+        <v>45.1</v>
       </c>
       <c r="D124">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -5264,13 +4970,13 @@
         <v>1220</v>
       </c>
       <c r="B125">
-        <v>447</v>
+        <v>44.7</v>
       </c>
       <c r="C125">
-        <v>452</v>
+        <v>45.2</v>
       </c>
       <c r="D125">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5279,13 +4985,13 @@
         <v>1230</v>
       </c>
       <c r="B126">
-        <v>448</v>
+        <v>44.8</v>
       </c>
       <c r="C126">
-        <v>448</v>
+        <v>44.8</v>
       </c>
       <c r="D126">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -5294,13 +5000,13 @@
         <v>1240</v>
       </c>
       <c r="B127">
-        <v>436</v>
+        <v>43.6</v>
       </c>
       <c r="C127">
-        <v>453</v>
+        <v>45.3</v>
       </c>
       <c r="D127">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5309,13 +5015,13 @@
         <v>1250</v>
       </c>
       <c r="B128">
-        <v>442</v>
+        <v>44.2</v>
       </c>
       <c r="C128">
-        <v>455</v>
+        <v>45.5</v>
       </c>
       <c r="D128">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5324,373 +5030,13 @@
         <v>1260</v>
       </c>
       <c r="B129">
-        <v>454</v>
+        <v>45.4</v>
       </c>
       <c r="C129">
-        <v>454</v>
+        <v>45.4</v>
       </c>
       <c r="D129">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <f t="shared" si="1"/>
-        <v>1270</v>
-      </c>
-      <c r="B130">
-        <v>446</v>
-      </c>
-      <c r="D130">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131">
-        <f t="shared" si="1"/>
-        <v>1280</v>
-      </c>
-      <c r="B131">
-        <v>445</v>
-      </c>
-      <c r="D131">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132">
-        <f t="shared" si="1"/>
-        <v>1290</v>
-      </c>
-      <c r="B132">
-        <v>452</v>
-      </c>
-      <c r="D132">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <f t="shared" si="1"/>
-        <v>1300</v>
-      </c>
-      <c r="B133">
-        <v>448</v>
-      </c>
-      <c r="D133">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <f t="shared" ref="A134:A159" si="2">A133+10</f>
-        <v>1310</v>
-      </c>
-      <c r="B134">
-        <v>448</v>
-      </c>
-      <c r="D134">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <f t="shared" si="2"/>
-        <v>1320</v>
-      </c>
-      <c r="B135">
-        <v>447</v>
-      </c>
-      <c r="D135">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <f t="shared" si="2"/>
-        <v>1330</v>
-      </c>
-      <c r="B136">
-        <v>456</v>
-      </c>
-      <c r="D136">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <f t="shared" si="2"/>
-        <v>1340</v>
-      </c>
-      <c r="B137">
-        <v>454</v>
-      </c>
-      <c r="D137">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <f t="shared" si="2"/>
-        <v>1350</v>
-      </c>
-      <c r="B138">
-        <v>456</v>
-      </c>
-      <c r="D138">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <f t="shared" si="2"/>
-        <v>1360</v>
-      </c>
-      <c r="B139">
-        <v>457</v>
-      </c>
-      <c r="D139">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <f t="shared" si="2"/>
-        <v>1370</v>
-      </c>
-      <c r="B140">
-        <v>458</v>
-      </c>
-      <c r="D140">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <f t="shared" si="2"/>
-        <v>1380</v>
-      </c>
-      <c r="B141">
-        <v>457</v>
-      </c>
-      <c r="D141">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <f t="shared" si="2"/>
-        <v>1390</v>
-      </c>
-      <c r="B142">
-        <v>459</v>
-      </c>
-      <c r="D142">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <f t="shared" si="2"/>
-        <v>1400</v>
-      </c>
-      <c r="B143">
-        <v>459</v>
-      </c>
-      <c r="D143">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <f t="shared" si="2"/>
-        <v>1410</v>
-      </c>
-      <c r="B144">
-        <v>460</v>
-      </c>
-      <c r="D144">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <f t="shared" si="2"/>
-        <v>1420</v>
-      </c>
-      <c r="B145">
-        <v>460</v>
-      </c>
-      <c r="D145">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <f t="shared" si="2"/>
-        <v>1430</v>
-      </c>
-      <c r="B146">
-        <v>463</v>
-      </c>
-      <c r="D146">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <f t="shared" si="2"/>
-        <v>1440</v>
-      </c>
-      <c r="B147">
-        <v>460</v>
-      </c>
-      <c r="D147">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <f t="shared" si="2"/>
-        <v>1450</v>
-      </c>
-      <c r="B148">
-        <v>460</v>
-      </c>
-      <c r="D148">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <f t="shared" si="2"/>
-        <v>1460</v>
-      </c>
-      <c r="B149">
-        <v>463</v>
-      </c>
-      <c r="D149">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <f t="shared" si="2"/>
-        <v>1470</v>
-      </c>
-      <c r="B150">
-        <v>466</v>
-      </c>
-      <c r="D150">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <f t="shared" si="2"/>
-        <v>1480</v>
-      </c>
-      <c r="B151">
-        <v>465</v>
-      </c>
-      <c r="D151">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <f t="shared" si="2"/>
-        <v>1490</v>
-      </c>
-      <c r="B152">
-        <v>458</v>
-      </c>
-      <c r="D152">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <f t="shared" si="2"/>
-        <v>1500</v>
-      </c>
-      <c r="B153">
-        <v>467</v>
-      </c>
-      <c r="D153">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <f t="shared" si="2"/>
-        <v>1510</v>
-      </c>
-      <c r="B154">
-        <v>463</v>
-      </c>
-      <c r="D154">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <f t="shared" si="2"/>
-        <v>1520</v>
-      </c>
-      <c r="B155">
-        <v>464</v>
-      </c>
-      <c r="D155">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156">
-        <f t="shared" si="2"/>
-        <v>1530</v>
-      </c>
-      <c r="B156">
-        <v>464</v>
-      </c>
-      <c r="D156">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157">
-        <f t="shared" si="2"/>
-        <v>1540</v>
-      </c>
-      <c r="B157">
-        <v>471</v>
-      </c>
-      <c r="D157">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158">
-        <f t="shared" si="2"/>
-        <v>1550</v>
-      </c>
-      <c r="B158">
-        <v>466</v>
-      </c>
-      <c r="D158">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159">
-        <f t="shared" si="2"/>
-        <v>1560</v>
-      </c>
-      <c r="B159">
-        <v>469</v>
-      </c>
-      <c r="D159">
-        <v>400</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>